<commit_message>
Continued work on a hue-shift spreadsheet.
</commit_message>
<xml_diff>
--- a/Workbench/hsv-diff-calculator.xlsx
+++ b/Workbench/hsv-diff-calculator.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workbench\gms2-akira-theme\Workbench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\GameMakerStudio2\Skins\Akira\Workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61B9DDC1-3A85-4CFC-9B22-92E9920FEEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36E633B-82FE-4B1B-93AE-A8368B7EEAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{33413FE7-37D2-47C7-85AF-7494BC4B024A}"/>
+    <workbookView xWindow="2895" yWindow="2955" windowWidth="18900" windowHeight="11055" xr2:uid="{33413FE7-37D2-47C7-85AF-7494BC4B024A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Hue</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Cursor/Pointer_No_5_5</t>
+  </si>
+  <si>
+    <t>Target Hue</t>
+  </si>
+  <si>
+    <t>Target Saturation</t>
+  </si>
+  <si>
+    <t>Target Value</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -116,22 +128,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15850C65-7102-488E-9963-76A36A6834E6}" name="Table1" displayName="Table1" ref="A2:G8" totalsRowShown="0">
-  <autoFilter ref="A2:G8" xr:uid="{877620F8-3A45-4472-998E-5436E10A0F7A}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{75ED0DBD-6264-46CF-B081-FC2AD119E6A5}" name="Color"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15850C65-7102-488E-9963-76A36A6834E6}" name="Table1" displayName="Table1" ref="A2:J7" totalsRowShown="0">
+  <autoFilter ref="A2:J7" xr:uid="{877620F8-3A45-4472-998E-5436E10A0F7A}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{75ED0DBD-6264-46CF-B081-FC2AD119E6A5}" name="Image"/>
     <tableColumn id="2" xr3:uid="{5AB3A1B4-1083-4B22-958C-CEEE60E8179C}" name="Hue"/>
     <tableColumn id="3" xr3:uid="{6A5EFE61-30F1-4880-A332-461B2A6C6548}" name="Saturation"/>
     <tableColumn id="4" xr3:uid="{FD2E54A7-4446-40C0-B157-8F096C542D94}" name="Value"/>
-    <tableColumn id="5" xr3:uid="{FDF3776E-77B4-4C06-8AF2-6DB511CAF691}" name="Hue Diff">
+    <tableColumn id="5" xr3:uid="{FDF3776E-77B4-4C06-8AF2-6DB511CAF691}" name="Target Hue">
       <calculatedColumnFormula>B3-B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DD5D412A-6A65-4691-80BE-2EBCAEFC49C9}" name="Saturation Diff">
+    <tableColumn id="6" xr3:uid="{DD5D412A-6A65-4691-80BE-2EBCAEFC49C9}" name="Target Saturation">
       <calculatedColumnFormula>C3-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{43626B23-3749-4F6C-978E-9F0C36C9EBD6}" name="Value Diff">
+    <tableColumn id="7" xr3:uid="{43626B23-3749-4F6C-978E-9F0C36C9EBD6}" name="Target Value">
       <calculatedColumnFormula>D3-D2</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="10" xr3:uid="{F7B92E3E-5F27-4F47-AAD6-772D7DDF95AC}" name="Hue Diff"/>
+    <tableColumn id="9" xr3:uid="{A8BE61A6-94CE-473E-8F8E-43FBF23A63B2}" name="Saturation Diff"/>
+    <tableColumn id="8" xr3:uid="{43B87188-044D-4DCF-A0EA-D2D1083AE9D1}" name="Value Diff"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1DA40E4-C005-473C-8BFB-4185778B5A20}" name="Table2" displayName="Table2" ref="L2:O8" totalsRowShown="0">
+  <autoFilter ref="L2:O8" xr:uid="{9D41AD28-CFE1-4524-B0B9-9F93E073133F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{97A15D29-23D6-4310-B33B-CB42DEC8FCEC}" name="Color"/>
+    <tableColumn id="2" xr3:uid="{866B11CF-20AE-4EBC-87BB-9037B014BE8F}" name="Hue"/>
+    <tableColumn id="3" xr3:uid="{A581280D-F788-47DD-8616-D160B72CF524}" name="Saturation"/>
+    <tableColumn id="4" xr3:uid="{DD1469D2-BA62-4B84-A669-DFA56D7B9E74}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,26 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EAC3CF-A5AD-4EB9-BBFE-84B1B8A50D18}">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -465,58 +494,70 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>179</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>85</v>
-      </c>
-      <c r="D3">
-        <v>88</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="C4">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <f>B4-$B$3</f>
-        <v>179</v>
-      </c>
-      <c r="F4">
-        <f>C4-$C$3</f>
-        <v>-15</v>
-      </c>
-      <c r="G4">
-        <f>D4-$D$3</f>
-        <v>12</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>128</v>
@@ -527,89 +568,26 @@
       <c r="D5">
         <v>83</v>
       </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E7" si="0">B5-$B$3</f>
-        <v>128</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F7" si="1">C5-$C$3</f>
-        <v>-17</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G7" si="2">D5-$D$3</f>
-        <v>-5</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>128</v>
+        <v>357</v>
       </c>
       <c r="C6">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D6">
-        <v>83</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>-17</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>357</v>
-      </c>
-      <c r="C7">
-        <v>82</v>
-      </c>
-      <c r="D7">
         <v>69</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>357</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="E8">
-        <f>B8-B7</f>
-        <v>-357</v>
-      </c>
-      <c r="F8">
-        <f>C8-C7</f>
-        <v>-82</v>
-      </c>
-      <c r="G8">
-        <f>D8-D7</f>
-        <v>-69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Shifted hues from stock dark theme to Akira palette colors...
But seriously, I have no idea what I'm doing.
</commit_message>
<xml_diff>
--- a/Workbench/hsv-diff-calculator.xlsx
+++ b/Workbench/hsv-diff-calculator.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\GameMakerStudio2\Skins\Akira\Workbench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workbench\gms2-akira-theme\Workbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36E633B-82FE-4B1B-93AE-A8368B7EEAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A857544D-F041-4B12-A752-A336435B3F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2955" windowWidth="18900" windowHeight="11055" xr2:uid="{33413FE7-37D2-47C7-85AF-7494BC4B024A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{33413FE7-37D2-47C7-85AF-7494BC4B024A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Hue</t>
   </si>
@@ -45,24 +45,9 @@
     <t>Value Diff</t>
   </si>
   <si>
-    <t>Akira Red</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
-    <t>Cursor/PointerBusy</t>
-  </si>
-  <si>
-    <t>Cursor/PointerGear</t>
-  </si>
-  <si>
-    <t>Cursor/PointerNewDesktop</t>
-  </si>
-  <si>
-    <t>Cursor/Pointer_No_5_5</t>
-  </si>
-  <si>
     <t>Target Hue</t>
   </si>
   <si>
@@ -72,7 +57,25 @@
     <t>Target Value</t>
   </si>
   <si>
-    <t>Image</t>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Maroon</t>
+  </si>
+  <si>
+    <t>Render</t>
   </si>
 </sst>
 </file>
@@ -88,12 +91,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE02121"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF105263"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9B3111"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B4353"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7EA328"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C2734"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,14 +147,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7C2734"/>
+      <color rgb="FF7EA328"/>
+      <color rgb="FF5B4353"/>
+      <color rgb="FF9B3111"/>
+      <color rgb="FF105263"/>
+      <color rgb="FFE02121"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -128,38 +183,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15850C65-7102-488E-9963-76A36A6834E6}" name="Table1" displayName="Table1" ref="A2:J7" totalsRowShown="0">
-  <autoFilter ref="A2:J7" xr:uid="{877620F8-3A45-4472-998E-5436E10A0F7A}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{75ED0DBD-6264-46CF-B081-FC2AD119E6A5}" name="Image"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15850C65-7102-488E-9963-76A36A6834E6}" name="Table1" displayName="Table1" ref="A2:I3" totalsRowShown="0">
+  <autoFilter ref="A2:I3" xr:uid="{877620F8-3A45-4472-998E-5436E10A0F7A}"/>
+  <tableColumns count="9">
     <tableColumn id="2" xr3:uid="{5AB3A1B4-1083-4B22-958C-CEEE60E8179C}" name="Hue"/>
     <tableColumn id="3" xr3:uid="{6A5EFE61-30F1-4880-A332-461B2A6C6548}" name="Saturation"/>
     <tableColumn id="4" xr3:uid="{FD2E54A7-4446-40C0-B157-8F096C542D94}" name="Value"/>
-    <tableColumn id="5" xr3:uid="{FDF3776E-77B4-4C06-8AF2-6DB511CAF691}" name="Target Hue">
-      <calculatedColumnFormula>B3-B2</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{FDF3776E-77B4-4C06-8AF2-6DB511CAF691}" name="Target Hue"/>
+    <tableColumn id="6" xr3:uid="{DD5D412A-6A65-4691-80BE-2EBCAEFC49C9}" name="Target Saturation"/>
+    <tableColumn id="7" xr3:uid="{43626B23-3749-4F6C-978E-9F0C36C9EBD6}" name="Target Value"/>
+    <tableColumn id="10" xr3:uid="{F7B92E3E-5F27-4F47-AAD6-772D7DDF95AC}" name="Hue Diff">
+      <calculatedColumnFormula>D3-A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DD5D412A-6A65-4691-80BE-2EBCAEFC49C9}" name="Target Saturation">
-      <calculatedColumnFormula>C3-C2</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{A8BE61A6-94CE-473E-8F8E-43FBF23A63B2}" name="Saturation Diff">
+      <calculatedColumnFormula>E3-B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{43626B23-3749-4F6C-978E-9F0C36C9EBD6}" name="Target Value">
-      <calculatedColumnFormula>D3-D2</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{43B87188-044D-4DCF-A0EA-D2D1083AE9D1}" name="Value Diff">
+      <calculatedColumnFormula>F3-C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F7B92E3E-5F27-4F47-AAD6-772D7DDF95AC}" name="Hue Diff"/>
-    <tableColumn id="9" xr3:uid="{A8BE61A6-94CE-473E-8F8E-43FBF23A63B2}" name="Saturation Diff"/>
-    <tableColumn id="8" xr3:uid="{43B87188-044D-4DCF-A0EA-D2D1083AE9D1}" name="Value Diff"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1DA40E4-C005-473C-8BFB-4185778B5A20}" name="Table2" displayName="Table2" ref="L2:O8" totalsRowShown="0">
-  <autoFilter ref="L2:O8" xr:uid="{9D41AD28-CFE1-4524-B0B9-9F93E073133F}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1DA40E4-C005-473C-8BFB-4185778B5A20}" name="Table2" displayName="Table2" ref="K2:O8" totalsRowShown="0">
+  <autoFilter ref="K2:O8" xr:uid="{9D41AD28-CFE1-4524-B0B9-9F93E073133F}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{97A15D29-23D6-4310-B33B-CB42DEC8FCEC}" name="Color"/>
     <tableColumn id="2" xr3:uid="{866B11CF-20AE-4EBC-87BB-9037B014BE8F}" name="Hue"/>
     <tableColumn id="3" xr3:uid="{A581280D-F788-47DD-8616-D160B72CF524}" name="Saturation"/>
     <tableColumn id="4" xr3:uid="{DD1469D2-BA62-4B84-A669-DFA56D7B9E74}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{612AC89B-F063-4ED5-BCFE-D20EE9635BD4}" name="Render"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,126 +517,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EAC3CF-A5AD-4EB9-BBFE-84B1B8A50D18}">
-  <dimension ref="A2:O6"/>
+  <dimension ref="A2:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>78</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>64</v>
+      </c>
+      <c r="G3">
+        <f>D3-A3</f>
+        <v>-53</v>
+      </c>
+      <c r="H3">
+        <f>E3-B3</f>
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <f>F3-C3</f>
+        <v>-4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>85</v>
+      </c>
+      <c r="N3">
+        <v>88</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>192</v>
+      </c>
+      <c r="M4">
+        <v>83</v>
+      </c>
+      <c r="N4">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="M5">
+        <v>89</v>
+      </c>
+      <c r="N5">
+        <v>61</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6">
+        <v>320</v>
+      </c>
+      <c r="M6">
+        <v>26</v>
+      </c>
+      <c r="N6">
+        <v>36</v>
+      </c>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7">
+        <v>78</v>
+      </c>
+      <c r="M7">
+        <v>75</v>
+      </c>
+      <c r="N7">
+        <v>64</v>
+      </c>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K8" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>179</v>
-      </c>
-      <c r="C3">
-        <v>70</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>128</v>
-      </c>
-      <c r="C4">
+      <c r="L8">
+        <v>351</v>
+      </c>
+      <c r="M8">
         <v>68</v>
       </c>
-      <c r="D4">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>128</v>
-      </c>
-      <c r="C5">
-        <v>68</v>
-      </c>
-      <c r="D5">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>357</v>
-      </c>
-      <c r="C6">
-        <v>82</v>
-      </c>
-      <c r="D6">
-        <v>69</v>
-      </c>
+      <c r="N8">
+        <v>49</v>
+      </c>
+      <c r="O8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>